<commit_message>
Remove unnecessary external link parsing in named range formulas.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/ExternalLinks.xlsx
+++ b/EPPlusTest/Workbooks/ExternalLinks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,6 +19,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="Named_Range">[1]Chart!$A$1</definedName>
+    <definedName name="OtherNamedRange">[1]Sheet1!XFA1048568</definedName>
   </definedNames>
   <calcPr calcId="162913" calcMode="manual" concurrentManualCount="1"/>
   <extLst>
@@ -110,6 +111,7 @@
     <sheetNames>
       <sheetName val="Chart"/>
       <sheetName val="Data"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -120,6 +122,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -391,7 +394,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +419,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <NimbusReport xmlns="http://JetReports/Nimbus/Schemas/2015/3" xmlns:i="http://www.w3.org/2001/XMLSchema-instance" xmlns:z="http://schemas.microsoft.com/2003/10/Serialization/" z:Id="1">
   <CalcChain z:Id="2">
     <Level>0</Level>
@@ -446,4 +449,14 @@
     </NimbusSheet>
   </mySheets>
 </NimbusReport>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DA72C6B-90A6-4DA2-85B5-5127D63ED743}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://JetReports/Nimbus/Schemas/2015/3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/2003/10/Serialization/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/2003/10/Serialization/Arrays"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>